<commit_message>
Matjaževi popravki glede baze.
</commit_message>
<xml_diff>
--- a/Podatki_za_v_bazo.xlsx
+++ b/Podatki_za_v_bazo.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15480" windowHeight="11640" tabRatio="898" firstSheet="17" activeTab="21"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15480" windowHeight="11640" tabRatio="898" firstSheet="14" activeTab="18"/>
   </bookViews>
   <sheets>
     <sheet name="Komentarji_vprašanja" sheetId="18" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3558" uniqueCount="1796">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3641" uniqueCount="1796">
   <si>
     <t>clani_skupine</t>
   </si>
@@ -5896,14 +5896,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G75"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -5913,9 +5914,8 @@
       <c r="B1" s="1" t="s">
         <v>845</v>
       </c>
-      <c r="C1" t="str">
-        <f>A1&amp;","&amp;B1</f>
-        <v>skupina,clan</v>
+      <c r="C1" t="s">
+        <v>852</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>846</v>
@@ -5928,6 +5928,9 @@
       <c r="B2" s="3" t="s">
         <v>25</v>
       </c>
+      <c r="C2" t="s">
+        <v>720</v>
+      </c>
       <c r="G2" t="s">
         <v>847</v>
       </c>
@@ -5939,6 +5942,9 @@
       <c r="B3" s="3" t="s">
         <v>26</v>
       </c>
+      <c r="C3" t="s">
+        <v>734</v>
+      </c>
       <c r="G3" t="s">
         <v>848</v>
       </c>
@@ -5950,6 +5956,9 @@
       <c r="B4" s="3" t="s">
         <v>27</v>
       </c>
+      <c r="C4" t="s">
+        <v>928</v>
+      </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" s="3" t="s">
@@ -5958,6 +5967,9 @@
       <c r="B5" s="3" t="s">
         <v>43</v>
       </c>
+      <c r="C5" t="s">
+        <v>928</v>
+      </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" s="3" t="s">
@@ -5966,6 +5978,9 @@
       <c r="B6" s="3" t="s">
         <v>29</v>
       </c>
+      <c r="C6" t="s">
+        <v>761</v>
+      </c>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" s="3" t="s">
@@ -5974,6 +5989,9 @@
       <c r="B7" s="3" t="s">
         <v>30</v>
       </c>
+      <c r="C7" t="s">
+        <v>741</v>
+      </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="3" t="s">
@@ -5982,6 +6000,9 @@
       <c r="B8" s="3" t="s">
         <v>31</v>
       </c>
+      <c r="C8" t="s">
+        <v>738</v>
+      </c>
     </row>
     <row r="9" spans="1:7">
       <c r="A9" s="3" t="s">
@@ -5990,6 +6011,9 @@
       <c r="B9" s="3" t="s">
         <v>32</v>
       </c>
+      <c r="C9" t="s">
+        <v>742</v>
+      </c>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" s="3" t="s">
@@ -5998,6 +6022,9 @@
       <c r="B10" s="3" t="s">
         <v>33</v>
       </c>
+      <c r="C10" t="s">
+        <v>928</v>
+      </c>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="3" t="s">
@@ -6006,6 +6033,9 @@
       <c r="B11" s="3" t="s">
         <v>34</v>
       </c>
+      <c r="C11" t="s">
+        <v>726</v>
+      </c>
     </row>
     <row r="12" spans="1:7">
       <c r="A12" s="3" t="s">
@@ -6014,6 +6044,9 @@
       <c r="B12" s="3" t="s">
         <v>35</v>
       </c>
+      <c r="C12" t="s">
+        <v>734</v>
+      </c>
     </row>
     <row r="13" spans="1:7">
       <c r="A13" s="3" t="s">
@@ -6022,6 +6055,9 @@
       <c r="B13" s="3" t="s">
         <v>36</v>
       </c>
+      <c r="C13" t="s">
+        <v>729</v>
+      </c>
     </row>
     <row r="14" spans="1:7">
       <c r="A14" s="3" t="s">
@@ -6030,6 +6066,9 @@
       <c r="B14" s="3" t="s">
         <v>37</v>
       </c>
+      <c r="C14" t="s">
+        <v>726</v>
+      </c>
     </row>
     <row r="15" spans="1:7">
       <c r="A15" s="3" t="s">
@@ -6038,6 +6077,9 @@
       <c r="B15" s="3" t="s">
         <v>38</v>
       </c>
+      <c r="C15" t="s">
+        <v>743</v>
+      </c>
     </row>
     <row r="16" spans="1:7">
       <c r="A16" s="3" t="s">
@@ -6046,477 +6088,657 @@
       <c r="B16" s="3" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="17" spans="1:2">
+      <c r="C16" t="s">
+        <v>726</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
       <c r="A17" s="3" t="s">
         <v>788</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="18" spans="1:2">
+      <c r="C17" t="s">
+        <v>764</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
       <c r="A18" s="3" t="s">
         <v>788</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="19" spans="1:2">
+      <c r="C18" t="s">
+        <v>765</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
       <c r="A19" s="3" t="s">
         <v>789</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="20" spans="1:2">
+      <c r="C19" t="s">
+        <v>763</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
       <c r="A20" s="3" t="s">
         <v>789</v>
       </c>
       <c r="B20" s="3" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="21" spans="1:2">
+      <c r="C20" t="s">
+        <v>928</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
       <c r="A21" s="3" t="s">
         <v>789</v>
       </c>
       <c r="B21" s="3" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="22" spans="1:2">
+      <c r="C21" t="s">
+        <v>726</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
       <c r="A22" s="3" t="s">
         <v>789</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="23" spans="1:2">
+      <c r="C22" t="s">
+        <v>726</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
       <c r="A23" s="3" t="s">
         <v>789</v>
       </c>
       <c r="B23" s="3" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="24" spans="1:2">
+      <c r="C23" t="s">
+        <v>726</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
       <c r="A24" s="3" t="s">
         <v>790</v>
       </c>
       <c r="B24" s="3" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="25" spans="1:2">
+      <c r="C24" t="s">
+        <v>741</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
       <c r="A25" s="3" t="s">
         <v>790</v>
       </c>
       <c r="B25" s="3" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="26" spans="1:2">
+      <c r="C25" t="s">
+        <v>735</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
       <c r="A26" s="3" t="s">
         <v>791</v>
       </c>
       <c r="B26" s="3" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="27" spans="1:2">
+      <c r="C26" t="s">
+        <v>739</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
       <c r="A27" s="3" t="s">
         <v>791</v>
       </c>
       <c r="B27" s="3" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="28" spans="1:2">
+      <c r="C27" t="s">
+        <v>710</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
       <c r="A28" s="3" t="s">
         <v>792</v>
       </c>
       <c r="B28" s="3" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="29" spans="1:2">
+      <c r="C28" t="s">
+        <v>737</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
       <c r="A29" s="3" t="s">
         <v>792</v>
       </c>
       <c r="B29" s="3" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="30" spans="1:2">
+      <c r="C29" t="s">
+        <v>726</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
       <c r="A30" s="3" t="s">
         <v>792</v>
       </c>
       <c r="B30" s="3" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="31" spans="1:2">
+      <c r="C30" t="s">
+        <v>729</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
       <c r="A31" s="3" t="s">
         <v>792</v>
       </c>
       <c r="B31" s="3" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="32" spans="1:2">
+      <c r="C31" t="s">
+        <v>726</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3">
       <c r="A32" s="3" t="s">
         <v>792</v>
       </c>
       <c r="B32" s="3" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="33" spans="1:2">
+      <c r="C32" t="s">
+        <v>741</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3">
       <c r="A33" s="3" t="s">
         <v>792</v>
       </c>
       <c r="B33" s="3" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="34" spans="1:2">
+      <c r="C33" t="s">
+        <v>729</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3">
       <c r="A34" s="3" t="s">
         <v>793</v>
       </c>
       <c r="B34" s="3" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="35" spans="1:2">
+      <c r="C34" t="s">
+        <v>741</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3">
       <c r="A35" s="3" t="s">
         <v>793</v>
       </c>
       <c r="B35" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="36" spans="1:2">
+      <c r="C35" t="s">
+        <v>726</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3">
       <c r="A36" s="3" t="s">
         <v>793</v>
       </c>
       <c r="B36" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="37" spans="1:2">
+      <c r="C36" t="s">
+        <v>928</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3">
       <c r="A37" s="3" t="s">
         <v>793</v>
       </c>
       <c r="B37" s="3" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="38" spans="1:2">
+      <c r="C37" t="s">
+        <v>726</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3">
       <c r="A38" s="3" t="s">
         <v>793</v>
       </c>
       <c r="B38" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="39" spans="1:2">
+      <c r="C38" t="s">
+        <v>928</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3">
       <c r="A39" s="3" t="s">
         <v>793</v>
       </c>
       <c r="B39" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="40" spans="1:2">
+      <c r="C39" t="s">
+        <v>742</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3">
       <c r="A40" s="3" t="s">
         <v>793</v>
       </c>
       <c r="B40" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="41" spans="1:2">
+      <c r="C40" t="s">
+        <v>741</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3">
       <c r="A41" s="3" t="s">
         <v>793</v>
       </c>
       <c r="B41" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="42" spans="1:2">
+      <c r="C41" t="s">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3">
       <c r="A42" s="3" t="s">
         <v>793</v>
       </c>
       <c r="B42" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="43" spans="1:2">
+      <c r="C42" t="s">
+        <v>713</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3">
       <c r="A43" s="3" t="s">
         <v>794</v>
       </c>
       <c r="B43" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="44" spans="1:2">
+      <c r="C43" t="s">
+        <v>729</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3">
       <c r="A44" s="3" t="s">
         <v>794</v>
       </c>
       <c r="B44" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="45" spans="1:2">
+      <c r="C44" t="s">
+        <v>726</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3">
       <c r="A45" s="3" t="s">
         <v>794</v>
       </c>
       <c r="B45" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="46" spans="1:2">
+      <c r="C45" t="s">
+        <v>733</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3">
       <c r="A46" s="3" t="s">
         <v>794</v>
       </c>
       <c r="B46" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="47" spans="1:2">
+      <c r="C46" t="s">
+        <v>735</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3">
       <c r="A47" s="3" t="s">
         <v>795</v>
       </c>
       <c r="B47" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="48" spans="1:2">
+      <c r="C47" t="s">
+        <v>726</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3">
       <c r="A48" s="3" t="s">
         <v>795</v>
       </c>
       <c r="B48" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="49" spans="1:2">
+      <c r="C48" t="s">
+        <v>730</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3">
       <c r="A49" s="3" t="s">
         <v>795</v>
       </c>
       <c r="B49" s="3" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="50" spans="1:2">
+      <c r="C49" t="s">
+        <v>928</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3">
       <c r="A50" s="3" t="s">
         <v>795</v>
       </c>
       <c r="B50" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="51" spans="1:2">
+      <c r="C50" t="s">
+        <v>738</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3">
       <c r="A51" s="3" t="s">
         <v>795</v>
       </c>
       <c r="B51" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="52" spans="1:2">
+      <c r="C51" t="s">
+        <v>726</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3">
       <c r="A52" s="3" t="s">
         <v>795</v>
       </c>
       <c r="B52" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="53" spans="1:2">
+      <c r="C52" t="s">
+        <v>928</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3">
       <c r="A53" s="3" t="s">
         <v>796</v>
       </c>
       <c r="B53" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="54" spans="1:2">
+      <c r="C53" t="s">
+        <v>928</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3">
       <c r="A54" s="3" t="s">
         <v>796</v>
       </c>
       <c r="B54" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="55" spans="1:2">
+      <c r="C54" t="s">
+        <v>928</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3">
       <c r="A55" s="3" t="s">
         <v>796</v>
       </c>
       <c r="B55" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="56" spans="1:2">
+      <c r="C55" t="s">
+        <v>928</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3">
       <c r="A56" s="3" t="s">
         <v>797</v>
       </c>
       <c r="B56" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="57" spans="1:2">
+      <c r="C56" t="s">
+        <v>729</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3">
       <c r="A57" s="3" t="s">
         <v>797</v>
       </c>
       <c r="B57" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="58" spans="1:2">
+      <c r="C57" t="s">
+        <v>726</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3">
       <c r="A58" s="3" t="s">
         <v>797</v>
       </c>
       <c r="B58" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="59" spans="1:2">
+      <c r="C58" t="s">
+        <v>928</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3">
       <c r="A59" s="3" t="s">
         <v>797</v>
       </c>
       <c r="B59" s="3" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="60" spans="1:2">
+      <c r="C59" t="s">
+        <v>726</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3">
       <c r="A60" s="3" t="s">
         <v>798</v>
       </c>
       <c r="B60" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="61" spans="1:2">
+      <c r="C60" t="s">
+        <v>736</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3">
       <c r="A61" s="3" t="s">
         <v>799</v>
       </c>
       <c r="B61" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="62" spans="1:2">
+      <c r="C61" t="s">
+        <v>726</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3">
       <c r="A62" s="3" t="s">
         <v>800</v>
       </c>
       <c r="B62" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="63" spans="1:2">
+      <c r="C62" t="s">
+        <v>731</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3">
       <c r="A63" s="3" t="s">
         <v>800</v>
       </c>
       <c r="B63" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="64" spans="1:2">
+      <c r="C63" t="s">
+        <v>732</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3">
       <c r="A64" s="3" t="s">
         <v>800</v>
       </c>
       <c r="B64" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="65" spans="1:2">
+      <c r="C64" t="s">
+        <v>726</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3">
       <c r="A65" s="3" t="s">
         <v>800</v>
       </c>
       <c r="B65" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="66" spans="1:2">
+      <c r="C65" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3">
       <c r="A66" s="3" t="s">
         <v>801</v>
       </c>
       <c r="B66" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="67" spans="1:2">
+      <c r="C66" t="s">
+        <v>766</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3">
       <c r="A67" s="3" t="s">
         <v>801</v>
       </c>
       <c r="B67" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="68" spans="1:2">
+      <c r="C67" t="s">
+        <v>726</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3">
       <c r="A68" s="3" t="s">
         <v>801</v>
       </c>
       <c r="B68" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="69" spans="1:2">
+      <c r="C68" t="s">
+        <v>726</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3">
       <c r="A69" s="3" t="s">
         <v>801</v>
       </c>
       <c r="B69" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="70" spans="1:2">
+      <c r="C69" t="s">
+        <v>928</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3">
       <c r="A70" s="3" t="s">
         <v>802</v>
       </c>
       <c r="B70" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="71" spans="1:2">
+      <c r="C70" t="s">
+        <v>740</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3">
       <c r="A71" s="3" t="s">
         <v>802</v>
       </c>
       <c r="B71" s="3" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="72" spans="1:2">
+      <c r="C71" t="s">
+        <v>928</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3">
       <c r="A72" s="3" t="s">
         <v>802</v>
       </c>
       <c r="B72" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="73" spans="1:2">
+      <c r="C72" t="s">
+        <v>768</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3">
       <c r="A73" s="3" t="s">
         <v>802</v>
       </c>
       <c r="B73" s="3" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="74" spans="1:2">
+      <c r="C73" t="s">
+        <v>726</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3">
       <c r="A74" s="3" t="s">
         <v>802</v>
       </c>
       <c r="B74" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="75" spans="1:2">
+      <c r="C74" t="s">
+        <v>729</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3">
       <c r="A75" s="3" t="s">
         <v>802</v>
       </c>
       <c r="B75" t="s">
         <v>99</v>
+      </c>
+      <c r="C75" t="s">
+        <v>726</v>
       </c>
     </row>
   </sheetData>
@@ -6529,7 +6751,7 @@
   <dimension ref="A1:F150"/>
   <sheetViews>
     <sheetView topLeftCell="A139" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="E57" sqref="E57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6933,7 +7155,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="49" spans="1:2">
+    <row r="49" spans="1:3">
       <c r="A49" t="s">
         <v>62</v>
       </c>
@@ -6941,7 +7163,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="50" spans="1:2">
+    <row r="50" spans="1:3">
       <c r="A50" t="s">
         <v>63</v>
       </c>
@@ -6949,7 +7171,7 @@
         <v>545</v>
       </c>
     </row>
-    <row r="51" spans="1:2">
+    <row r="51" spans="1:3">
       <c r="A51" t="s">
         <v>28</v>
       </c>
@@ -6957,7 +7179,7 @@
         <v>607</v>
       </c>
     </row>
-    <row r="52" spans="1:2">
+    <row r="52" spans="1:3">
       <c r="A52" t="s">
         <v>28</v>
       </c>
@@ -6965,7 +7187,7 @@
         <v>623</v>
       </c>
     </row>
-    <row r="53" spans="1:2">
+    <row r="53" spans="1:3">
       <c r="A53" t="s">
         <v>64</v>
       </c>
@@ -6973,15 +7195,18 @@
         <v>543</v>
       </c>
     </row>
-    <row r="54" spans="1:2">
+    <row r="54" spans="1:3">
       <c r="A54" t="s">
         <v>65</v>
       </c>
       <c r="B54" t="s">
         <v>605</v>
       </c>
-    </row>
-    <row r="55" spans="1:2">
+      <c r="C54" t="s">
+        <v>928</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3">
       <c r="A55" t="s">
         <v>66</v>
       </c>
@@ -6989,7 +7214,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="56" spans="1:2">
+    <row r="56" spans="1:3">
       <c r="A56" t="s">
         <v>67</v>
       </c>
@@ -6997,7 +7222,7 @@
         <v>572</v>
       </c>
     </row>
-    <row r="57" spans="1:2">
+    <row r="57" spans="1:3">
       <c r="A57" t="s">
         <v>67</v>
       </c>
@@ -7005,7 +7230,7 @@
         <v>622</v>
       </c>
     </row>
-    <row r="58" spans="1:2">
+    <row r="58" spans="1:3">
       <c r="A58" t="s">
         <v>68</v>
       </c>
@@ -7013,7 +7238,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="59" spans="1:2">
+    <row r="59" spans="1:3">
       <c r="A59" t="s">
         <v>68</v>
       </c>
@@ -7021,7 +7246,7 @@
         <v>620</v>
       </c>
     </row>
-    <row r="60" spans="1:2">
+    <row r="60" spans="1:3">
       <c r="A60" t="s">
         <v>69</v>
       </c>
@@ -7029,7 +7254,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="61" spans="1:2">
+    <row r="61" spans="1:3">
       <c r="A61" t="s">
         <v>70</v>
       </c>
@@ -7037,7 +7262,7 @@
         <v>535</v>
       </c>
     </row>
-    <row r="62" spans="1:2">
+    <row r="62" spans="1:3">
       <c r="A62" t="s">
         <v>71</v>
       </c>
@@ -7045,7 +7270,7 @@
         <v>579</v>
       </c>
     </row>
-    <row r="63" spans="1:2">
+    <row r="63" spans="1:3">
       <c r="A63" t="s">
         <v>72</v>
       </c>
@@ -7053,7 +7278,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="64" spans="1:2">
+    <row r="64" spans="1:3">
       <c r="A64" t="s">
         <v>72</v>
       </c>
@@ -12791,10 +13016,10 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E97"/>
+  <dimension ref="A1:E100"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView topLeftCell="A91" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H93" sqref="H93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -14167,8 +14392,51 @@
         <v>1985</v>
       </c>
     </row>
+    <row r="98" spans="1:4">
+      <c r="A98" t="s">
+        <v>25</v>
+      </c>
+      <c r="B98" t="s">
+        <v>720</v>
+      </c>
+      <c r="C98" t="s">
+        <v>1795</v>
+      </c>
+      <c r="D98">
+        <v>2006</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4">
+      <c r="A99" t="s">
+        <v>38</v>
+      </c>
+      <c r="B99" t="s">
+        <v>743</v>
+      </c>
+      <c r="C99" t="s">
+        <v>702</v>
+      </c>
+      <c r="D99">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4">
+      <c r="A100" t="s">
+        <v>65</v>
+      </c>
+      <c r="B100" t="s">
+        <v>705</v>
+      </c>
+      <c r="C100" t="s">
+        <v>702</v>
+      </c>
+      <c r="D100">
+        <v>2003</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -14176,7 +14444,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D59"/>
   <sheetViews>
-    <sheetView topLeftCell="A52" workbookViewId="0">
+    <sheetView topLeftCell="A25" workbookViewId="0">
       <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
@@ -15816,7 +16084,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="C2" sqref="C2:C36"/>
     </sheetView>
   </sheetViews>
@@ -16125,9 +16393,9 @@
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E20"/>
+  <dimension ref="A1:E19"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
       <selection activeCell="A20" sqref="A20:D20"/>
     </sheetView>
   </sheetViews>
@@ -16405,20 +16673,6 @@
         <v>700</v>
       </c>
       <c r="D19">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4">
-      <c r="A20" t="s">
-        <v>794</v>
-      </c>
-      <c r="B20" t="s">
-        <v>928</v>
-      </c>
-      <c r="C20" t="s">
-        <v>699</v>
-      </c>
-      <c r="D20">
         <v>1</v>
       </c>
     </row>
@@ -19562,7 +19816,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
@@ -20018,7 +20272,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
@@ -20274,13 +20528,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="2.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5" style="3" customWidth="1"/>
     <col min="2" max="2" width="22" style="3" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18.5703125" style="3" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.5703125" style="3" bestFit="1" customWidth="1"/>
@@ -22103,10 +22357,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H21"/>
+  <dimension ref="A1:H54"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection activeCell="E57" sqref="E57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -22564,6 +22818,12 @@
         <v>734036380</v>
       </c>
     </row>
+    <row r="54" spans="3:4">
+      <c r="C54" t="s">
+        <v>928</v>
+      </c>
+      <c r="D54"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>